<commit_message>
Doku & Gant 2.0
</commit_message>
<xml_diff>
--- a/Dokumentation/GanttDiagramm.xlsx
+++ b/Dokumentation/GanttDiagramm.xlsx
@@ -384,7 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
@@ -451,23 +451,30 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -487,31 +494,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -968,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN1654"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ54" sqref="AJ54"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,58 +1032,58 @@
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="43"/>
       <c r="C1" s="13"/>
       <c r="D1" s="14"/>
       <c r="E1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="17"/>
-      <c r="G1" s="56">
+      <c r="G1" s="39">
         <v>18.5</v>
       </c>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="56">
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="39">
         <v>1.6</v>
       </c>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="56">
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="39">
         <v>8.6</v>
       </c>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="56">
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="39">
         <v>15.6</v>
       </c>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="56">
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="39">
         <v>22.6</v>
       </c>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="56">
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="39">
         <v>29.6</v>
       </c>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="57"/>
-      <c r="AJ1" s="57"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
     </row>
     <row r="2" spans="1:47" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="53"/>
+      <c r="B2" s="43"/>
       <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
@@ -1183,15 +1184,15 @@
       </c>
     </row>
     <row r="3" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="23"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
       <c r="F3" s="20" t="s">
         <v>5</v>
       </c>
@@ -1210,11 +1211,11 @@
       <c r="AI3" s="8"/>
     </row>
     <row r="4" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="21" t="s">
         <v>6</v>
       </c>
@@ -1247,13 +1248,13 @@
       <c r="AU4" s="22"/>
     </row>
     <row r="5" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="23"/>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="20" t="s">
         <v>5</v>
       </c>
@@ -1272,11 +1273,11 @@
       <c r="AI5" s="8"/>
     </row>
     <row r="6" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="21" t="s">
         <v>6</v>
       </c>
@@ -1307,13 +1308,13 @@
       <c r="AU6" s="22"/>
     </row>
     <row r="7" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="20" t="s">
         <v>5</v>
       </c>
@@ -1333,11 +1334,11 @@
       <c r="AI7" s="8"/>
     </row>
     <row r="8" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="42"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="21" t="s">
         <v>6</v>
       </c>
@@ -1367,13 +1368,13 @@
       <c r="AU8" s="22"/>
     </row>
     <row r="9" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="20" t="s">
         <v>5</v>
       </c>
@@ -1391,11 +1392,11 @@
       <c r="AI9" s="8"/>
     </row>
     <row r="10" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="23"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="21" t="s">
         <v>6</v>
       </c>
@@ -1425,13 +1426,13 @@
       <c r="AU10" s="22"/>
     </row>
     <row r="11" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="23"/>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="20" t="s">
         <v>5</v>
       </c>
@@ -1449,11 +1450,11 @@
       <c r="AI11" s="8"/>
     </row>
     <row r="12" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="21" t="s">
         <v>6</v>
       </c>
@@ -1483,13 +1484,13 @@
       <c r="AU12" s="22"/>
     </row>
     <row r="13" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="23"/>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="20" t="s">
         <v>5</v>
       </c>
@@ -1507,11 +1508,11 @@
       <c r="AI13" s="8"/>
     </row>
     <row r="14" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="42"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="23"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="21" t="s">
         <v>6</v>
       </c>
@@ -1547,13 +1548,13 @@
       <c r="AU14" s="22"/>
     </row>
     <row r="15" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="20" t="s">
         <v>5</v>
       </c>
@@ -1576,11 +1577,11 @@
       <c r="AI15" s="8"/>
     </row>
     <row r="16" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42"/>
+      <c r="A16" s="54"/>
       <c r="B16" s="23"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="21" t="s">
         <v>6</v>
       </c>
@@ -1611,13 +1612,13 @@
       <c r="AU16" s="22"/>
     </row>
     <row r="17" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="23"/>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="20" t="s">
         <v>5</v>
       </c>
@@ -1628,6 +1629,7 @@
       <c r="T17" s="28"/>
       <c r="U17" s="8"/>
       <c r="V17" s="6"/>
+      <c r="X17" s="59"/>
       <c r="Z17" s="8"/>
       <c r="AA17" s="6"/>
       <c r="AE17" s="8"/>
@@ -1635,11 +1637,11 @@
       <c r="AI17" s="8"/>
     </row>
     <row r="18" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="21" t="s">
         <v>6</v>
       </c>
@@ -1669,15 +1671,15 @@
       <c r="AU18" s="22"/>
     </row>
     <row r="19" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="53" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="23"/>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="20" t="s">
         <v>5</v>
       </c>
@@ -1697,11 +1699,11 @@
       <c r="AI19" s="8"/>
     </row>
     <row r="20" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="21" t="s">
         <v>6</v>
       </c>
@@ -1732,13 +1734,13 @@
       <c r="AU20" s="22"/>
     </row>
     <row r="21" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
       <c r="F21" s="20" t="s">
         <v>5</v>
       </c>
@@ -1756,11 +1758,11 @@
       <c r="AI21" s="8"/>
     </row>
     <row r="22" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="23"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="21" t="s">
         <v>6</v>
       </c>
@@ -1792,13 +1794,13 @@
       <c r="AU22" s="22"/>
     </row>
     <row r="23" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="23"/>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="38"/>
-      <c r="E23" s="50"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="56"/>
       <c r="F23" s="20" t="s">
         <v>5</v>
       </c>
@@ -1816,11 +1818,11 @@
       <c r="AI23" s="8"/>
     </row>
     <row r="24" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="42"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="51"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="57"/>
       <c r="F24" s="21" t="s">
         <v>6</v>
       </c>
@@ -1853,13 +1855,13 @@
       <c r="AU24" s="22"/>
     </row>
     <row r="25" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="45"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="20" t="s">
         <v>5</v>
       </c>
@@ -1879,11 +1881,11 @@
       <c r="AI25" s="8"/>
     </row>
     <row r="26" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="42"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="23"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="47"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="21" t="s">
         <v>6</v>
       </c>
@@ -1913,13 +1915,13 @@
       <c r="AU26" s="22"/>
     </row>
     <row r="27" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="42"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="48"/>
       <c r="F27" s="20" t="s">
         <v>5</v>
       </c>
@@ -1939,11 +1941,11 @@
       <c r="AI27" s="8"/>
     </row>
     <row r="28" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="42"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="23"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="47"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="50"/>
       <c r="F28" s="21" t="s">
         <v>6</v>
       </c>
@@ -1973,13 +1975,13 @@
       <c r="AU28" s="22"/>
     </row>
     <row r="29" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="42"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="23"/>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="48"/>
       <c r="F29" s="20" t="s">
         <v>5</v>
       </c>
@@ -1999,11 +2001,11 @@
       <c r="AI29" s="8"/>
     </row>
     <row r="30" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="42"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="47"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="50"/>
       <c r="F30" s="21" t="s">
         <v>6</v>
       </c>
@@ -2033,13 +2035,13 @@
       <c r="AU30" s="22"/>
     </row>
     <row r="31" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="23"/>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="44"/>
-      <c r="E31" s="45"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="48"/>
       <c r="F31" s="20" t="s">
         <v>5</v>
       </c>
@@ -2059,11 +2061,11 @@
       <c r="AI31" s="8"/>
     </row>
     <row r="32" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="23"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="47"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="50"/>
       <c r="F32" s="21" t="s">
         <v>6</v>
       </c>
@@ -2093,13 +2095,13 @@
       <c r="AU32" s="22"/>
     </row>
     <row r="33" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="42"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="23"/>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="45"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="48"/>
       <c r="F33" s="20" t="s">
         <v>5</v>
       </c>
@@ -2117,11 +2119,11 @@
       <c r="AI33" s="8"/>
     </row>
     <row r="34" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
+      <c r="A34" s="54"/>
       <c r="B34" s="23"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="47"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
       <c r="F34" s="21" t="s">
         <v>6</v>
       </c>
@@ -2151,13 +2153,13 @@
       <c r="AU34" s="22"/>
     </row>
     <row r="35" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="42"/>
+      <c r="A35" s="54"/>
       <c r="B35" s="23"/>
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="44"/>
-      <c r="E35" s="45"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="48"/>
       <c r="F35" s="20" t="s">
         <v>5</v>
       </c>
@@ -2175,11 +2177,11 @@
       <c r="AI35" s="8"/>
     </row>
     <row r="36" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="42"/>
+      <c r="A36" s="54"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="47"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="50"/>
       <c r="F36" s="21" t="s">
         <v>6</v>
       </c>
@@ -2209,13 +2211,13 @@
       <c r="AU36" s="22"/>
     </row>
     <row r="37" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
+      <c r="A37" s="54"/>
       <c r="B37" s="23"/>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="44"/>
-      <c r="E37" s="45"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="48"/>
       <c r="F37" s="20" t="s">
         <v>5</v>
       </c>
@@ -2235,11 +2237,11 @@
       <c r="AI37" s="29"/>
     </row>
     <row r="38" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="43"/>
+      <c r="A38" s="55"/>
       <c r="B38" s="23"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="47"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="50"/>
       <c r="F38" s="21" t="s">
         <v>6</v>
       </c>
@@ -2269,15 +2271,15 @@
       <c r="AU38" s="22"/>
     </row>
     <row r="39" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="41" t="s">
+      <c r="A39" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="40"/>
-      <c r="C39" s="38" t="s">
+      <c r="B39" s="58"/>
+      <c r="C39" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="44"/>
-      <c r="E39" s="45"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="48"/>
       <c r="F39" s="20" t="s">
         <v>5</v>
       </c>
@@ -2295,11 +2297,11 @@
       <c r="AI39" s="8"/>
     </row>
     <row r="40" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="42"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="47"/>
+      <c r="A40" s="54"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="50"/>
       <c r="F40" s="21" t="s">
         <v>6</v>
       </c>
@@ -2329,13 +2331,13 @@
       <c r="AU40" s="22"/>
     </row>
     <row r="41" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="42"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="48" t="s">
+      <c r="A41" s="54"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="44"/>
-      <c r="E41" s="45"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="48"/>
       <c r="F41" s="20" t="s">
         <v>5</v>
       </c>
@@ -2353,11 +2355,11 @@
       <c r="AI41" s="8"/>
     </row>
     <row r="42" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="42"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="47"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="50"/>
       <c r="F42" s="21" t="s">
         <v>6</v>
       </c>
@@ -2387,13 +2389,13 @@
       <c r="AU42" s="22"/>
     </row>
     <row r="43" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="42"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="38" t="s">
+      <c r="A43" s="54"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="45"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="48"/>
       <c r="F43" s="20" t="s">
         <v>5</v>
       </c>
@@ -2412,11 +2414,11 @@
       <c r="AI43" s="8"/>
     </row>
     <row r="44" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="43"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="47"/>
+      <c r="A44" s="55"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="50"/>
       <c r="F44" s="21" t="s">
         <v>6</v>
       </c>
@@ -2446,15 +2448,15 @@
       <c r="AU44" s="22"/>
     </row>
     <row r="45" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="48" t="s">
+      <c r="B45" s="58"/>
+      <c r="C45" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="44"/>
-      <c r="E45" s="45"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="48"/>
       <c r="F45" s="20" t="s">
         <v>5</v>
       </c>
@@ -2474,11 +2476,11 @@
       <c r="AI45" s="29"/>
     </row>
     <row r="46" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="42"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="47"/>
+      <c r="A46" s="54"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="50"/>
       <c r="F46" s="21" t="s">
         <v>6</v>
       </c>
@@ -2494,7 +2496,7 @@
       <c r="AE46" s="11"/>
       <c r="AF46" s="9"/>
       <c r="AI46" s="11"/>
-      <c r="AJ46" s="58"/>
+      <c r="AJ46" s="38"/>
       <c r="AK46" s="22"/>
       <c r="AL46" s="22"/>
       <c r="AM46" s="22"/>
@@ -2508,13 +2510,13 @@
       <c r="AU46" s="22"/>
     </row>
     <row r="47" spans="1:47" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="42"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="48" t="s">
+      <c r="A47" s="54"/>
+      <c r="B47" s="58"/>
+      <c r="C47" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D47" s="44"/>
-      <c r="E47" s="45"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="48"/>
       <c r="F47" s="20" t="s">
         <v>5</v>
       </c>
@@ -2534,11 +2536,11 @@
       <c r="AI47" s="29"/>
     </row>
     <row r="48" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="42"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="47"/>
+      <c r="A48" s="54"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="50"/>
       <c r="F48" s="21" t="s">
         <v>6</v>
       </c>
@@ -2554,7 +2556,7 @@
       <c r="AE48" s="11"/>
       <c r="AF48" s="9"/>
       <c r="AI48" s="11"/>
-      <c r="AJ48" s="58"/>
+      <c r="AJ48" s="38"/>
       <c r="AK48" s="22"/>
       <c r="AL48" s="22"/>
       <c r="AM48" s="22"/>
@@ -2568,13 +2570,13 @@
       <c r="AU48" s="22"/>
     </row>
     <row r="49" spans="1:66" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="42"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="48" t="s">
+      <c r="A49" s="54"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="D49" s="44"/>
-      <c r="E49" s="45"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="48"/>
       <c r="F49" s="20" t="s">
         <v>5</v>
       </c>
@@ -2594,11 +2596,11 @@
       <c r="AI49" s="29"/>
     </row>
     <row r="50" spans="1:66" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="42"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="47"/>
+      <c r="A50" s="54"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="50"/>
       <c r="F50" s="21" t="s">
         <v>6</v>
       </c>
@@ -2614,7 +2616,7 @@
       <c r="AE50" s="11"/>
       <c r="AF50" s="9"/>
       <c r="AI50" s="11"/>
-      <c r="AJ50" s="58"/>
+      <c r="AJ50" s="38"/>
       <c r="AK50" s="22"/>
       <c r="AL50" s="22"/>
       <c r="AM50" s="22"/>
@@ -2628,13 +2630,13 @@
       <c r="AU50" s="22"/>
     </row>
     <row r="51" spans="1:66" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="42"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="48" t="s">
+      <c r="A51" s="54"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D51" s="44"/>
-      <c r="E51" s="45"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="48"/>
       <c r="F51" s="20" t="s">
         <v>5</v>
       </c>
@@ -2654,11 +2656,11 @@
       <c r="AI51" s="29"/>
     </row>
     <row r="52" spans="1:66" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="42"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="47"/>
+      <c r="A52" s="54"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="50"/>
       <c r="F52" s="21" t="s">
         <v>6</v>
       </c>
@@ -2674,7 +2676,7 @@
       <c r="AE52" s="11"/>
       <c r="AF52" s="9"/>
       <c r="AI52" s="11"/>
-      <c r="AJ52" s="58"/>
+      <c r="AJ52" s="38"/>
       <c r="AK52" s="22"/>
       <c r="AL52" s="22"/>
       <c r="AM52" s="22"/>
@@ -2707,13 +2709,13 @@
       <c r="BN52" s="22"/>
     </row>
     <row r="53" spans="1:66" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="42"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="38" t="s">
+      <c r="A53" s="54"/>
+      <c r="B53" s="58"/>
+      <c r="C53" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="44"/>
-      <c r="E53" s="45"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="48"/>
       <c r="F53" s="20" t="s">
         <v>5</v>
       </c>
@@ -2733,11 +2735,11 @@
       <c r="AI53" s="29"/>
     </row>
     <row r="54" spans="1:66" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="43"/>
-      <c r="B54" s="40"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="47"/>
+      <c r="A54" s="55"/>
+      <c r="B54" s="58"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="50"/>
       <c r="F54" s="24" t="s">
         <v>6</v>
       </c>
@@ -2753,7 +2755,7 @@
       <c r="AE54" s="26"/>
       <c r="AF54" s="25"/>
       <c r="AI54" s="26"/>
-      <c r="AJ54" s="58"/>
+      <c r="AJ54" s="38"/>
     </row>
     <row r="55" spans="1:66" x14ac:dyDescent="0.3">
       <c r="J55" s="4"/>
@@ -57157,31 +57159,30 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AE1"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:E6"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D37:E38"/>
-    <mergeCell ref="D39:E40"/>
-    <mergeCell ref="D29:E30"/>
-    <mergeCell ref="D31:E32"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="B45:B54"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A45:A54"/>
+    <mergeCell ref="D41:E42"/>
+    <mergeCell ref="D53:E54"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D49:E50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:E52"/>
+    <mergeCell ref="D43:E44"/>
+    <mergeCell ref="D45:E46"/>
+    <mergeCell ref="D47:E48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
     <mergeCell ref="A19:A38"/>
     <mergeCell ref="A3:A18"/>
     <mergeCell ref="D33:E34"/>
@@ -57198,30 +57199,31 @@
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D7:E8"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A45:A54"/>
-    <mergeCell ref="D41:E42"/>
-    <mergeCell ref="D53:E54"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D49:E50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:E52"/>
-    <mergeCell ref="D43:E44"/>
-    <mergeCell ref="D45:E46"/>
-    <mergeCell ref="D47:E48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B39:B44"/>
-    <mergeCell ref="B45:B54"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D37:E38"/>
+    <mergeCell ref="D39:E40"/>
+    <mergeCell ref="D29:E30"/>
+    <mergeCell ref="D31:E32"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AE1"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>